<commit_message>
up to 9/9 (fixed workbook links)
</commit_message>
<xml_diff>
--- a/daily_logs.xlsx
+++ b/daily_logs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johntomczak\Desktop\market_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JohnTomczak/Documents/work/finance/numbers/market_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12440" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="all_markets" sheetId="8" r:id="rId1"/>
@@ -21,11 +21,11 @@
     <sheet name="data" sheetId="2" r:id="rId7"/>
     <sheet name="fidelity" sheetId="6" r:id="rId8"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -365,66 +365,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="all_markets"/>
-      <sheetName val="stocks"/>
-      <sheetName val="currencies"/>
-      <sheetName val="commodities"/>
-      <sheetName val="fixed_income"/>
-      <sheetName val="FedWatch"/>
-      <sheetName val="data"/>
-      <sheetName val="fidelity"/>
-      <sheetName val="VIX_SPX"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>S&amp;P 500</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>42611</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>42612</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>42613</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>42614</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>42615</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -692,11 +632,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView showFormulas="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1866,7 +1806,7 @@
       <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2170,10 +2110,10 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2256,12 +2196,12 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2283,7 +2223,6 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <f>[1]stocks!A2</f>
         <v>42611</v>
       </c>
       <c r="B2" s="3">
@@ -2302,7 +2241,6 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <f>[1]stocks!A3</f>
         <v>42612</v>
       </c>
       <c r="B3" s="3">
@@ -2321,7 +2259,6 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f>[1]stocks!A4</f>
         <v>42613</v>
       </c>
       <c r="B4" s="3">
@@ -2340,7 +2277,6 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f>[1]stocks!A5</f>
         <v>42614</v>
       </c>
       <c r="B5" s="3">
@@ -2359,7 +2295,6 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f>[1]stocks!A6</f>
         <v>42615</v>
       </c>
       <c r="B6" s="3">
@@ -2458,10 +2393,10 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A10"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2506,7 +2441,6 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <f>[1]stocks!A2</f>
         <v>42611</v>
       </c>
       <c r="B2" s="3">
@@ -2545,7 +2479,6 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <f>[1]stocks!A3</f>
         <v>42612</v>
       </c>
       <c r="B3" s="3">
@@ -2584,7 +2517,6 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f>[1]stocks!A4</f>
         <v>42613</v>
       </c>
       <c r="B4" s="3">
@@ -2863,7 +2795,7 @@
       <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
@@ -3330,7 +3262,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -3343,7 +3275,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -3356,10 +3288,10 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>49</v>
       </c>
@@ -3391,7 +3323,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -3404,7 +3336,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -3417,7 +3349,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -3430,7 +3362,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -3443,7 +3375,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -3456,7 +3388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3469,7 +3401,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>50</v>
       </c>
@@ -3501,7 +3433,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -3514,7 +3446,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -3527,7 +3459,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -3540,7 +3472,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -3553,7 +3485,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -3566,7 +3498,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -3588,14 +3520,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="6" max="6" width="11.25" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3911,11 +3843,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3934,7 +3866,6 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <f>stocks!A2</f>
         <v>42611</v>
       </c>
       <c r="B2" s="3">
@@ -3949,7 +3880,6 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <f>stocks!A3</f>
         <v>42612</v>
       </c>
       <c r="B3" s="3">
@@ -3964,7 +3894,6 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f>stocks!A4</f>
         <v>42613</v>
       </c>
       <c r="B4" s="3">

</xml_diff>

<commit_message>
up to 9/9 (final data push)
This is as far as I got with the bbg terminal.
I accidentally overwrote and lost the FX data, so I need to update that
at a later time. This is the 3rd push of essentially the same numbers,
due to me having to fix some links and learning the Desktop app.
</commit_message>
<xml_diff>
--- a/daily_logs.xlsx
+++ b/daily_logs.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JohnTomczak/Documents/work/finance/numbers/market_logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johntomczak\Desktop\market_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12440" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="12435" tabRatio="500" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="all_markets" sheetId="8" r:id="rId1"/>
@@ -21,11 +21,8 @@
     <sheet name="data" sheetId="2" r:id="rId7"/>
     <sheet name="fidelity" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -636,7 +633,7 @@
       <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1806,7 +1803,7 @@
       <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2113,7 +2110,7 @@
       <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2199,9 +2196,9 @@
       <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2396,7 +2393,7 @@
       <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2795,9 +2792,9 @@
       <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>43</v>
       </c>
@@ -2829,7 +2826,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -2842,7 +2839,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -2855,7 +2852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>44</v>
       </c>
@@ -2887,7 +2884,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -2900,7 +2897,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -2913,7 +2910,7 @@
         <v>32.6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -2926,7 +2923,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
@@ -2958,7 +2955,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2971,7 +2968,7 @@
         <v>39.6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2984,7 +2981,7 @@
         <v>45.6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -2997,7 +2994,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -3010,7 +3007,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>46</v>
       </c>
@@ -3042,7 +3039,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -3055,7 +3052,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -3068,7 +3065,7 @@
         <v>45.2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -3081,7 +3078,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -3094,7 +3091,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>47</v>
       </c>
@@ -3126,7 +3123,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -3139,7 +3136,7 @@
         <v>31.3</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -3152,7 +3149,7 @@
         <v>43.9</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -3165,7 +3162,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -3178,7 +3175,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -3191,7 +3188,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>48</v>
       </c>
@@ -3223,7 +3220,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -3236,7 +3233,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -3249,7 +3246,7 @@
         <v>43.4</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -3262,7 +3259,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -3275,7 +3272,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -3288,10 +3285,10 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>49</v>
       </c>
@@ -3323,7 +3320,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -3336,7 +3333,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -3349,7 +3346,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -3362,7 +3359,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -3375,7 +3372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -3388,7 +3385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3401,7 +3398,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>50</v>
       </c>
@@ -3433,7 +3430,7 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -3446,7 +3443,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>38</v>
       </c>
@@ -3459,7 +3456,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -3472,7 +3469,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -3485,7 +3482,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -3498,7 +3495,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -3524,10 +3521,10 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3844,10 +3841,10 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>